<commit_message>
GUI PRE-PROTOTYPE BACKUP v.2
add Skill
</commit_message>
<xml_diff>
--- a/TestConsoleClient/TestConsoleClient/res/card.xlsx
+++ b/TestConsoleClient/TestConsoleClient/res/card.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -112,9 +113,6 @@
     <t>서큐버스 퀸의 유혹</t>
   </si>
   <si>
-    <t>전장에 나와 있는 적군 중 하나를 아군으로 만든다.</t>
-  </si>
-  <si>
     <r>
       <t>n</t>
     </r>
@@ -561,37 +559,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>드래곤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미니언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>imited_amount</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전장에 나와 있는 적군 중 하나를 아군으로 만든다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>전장에서 카드가 하나 파괴 될 때마다 플레이어의 생명력이 +1 된다. 이효과는 이 카드가 파괴 될때까지 지속 되며 자기 자신의 파괴는 포함하지 않는다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드래곤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미니언</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>imited_amount</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -638,7 +640,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +656,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -708,6 +716,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1014,7 +1025,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1035,49 +1046,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1088,19 +1099,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -1118,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -1131,19 +1142,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1161,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1174,19 +1185,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -1217,19 +1228,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1247,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1260,19 +1271,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -1290,7 +1301,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1300,22 +1311,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -1333,7 +1344,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1346,19 +1357,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -1389,19 +1400,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="1">
         <v>6</v>
@@ -1418,8 +1429,8 @@
       <c r="L9" s="4">
         <v>8</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>73</v>
+      <c r="M9" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1432,19 +1443,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="1">
         <v>6</v>
@@ -1475,19 +1486,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1505,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1518,19 +1529,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1">
         <v>5</v>
@@ -1561,19 +1572,19 @@
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1591,7 +1602,7 @@
         <v>12</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1604,19 +1615,19 @@
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1">
         <v>4</v>
@@ -1647,19 +1658,19 @@
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1">
         <v>3</v>
@@ -1677,7 +1688,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1690,19 +1701,19 @@
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1">
         <v>5</v>
@@ -1720,7 +1731,7 @@
         <v>15</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1733,19 +1744,19 @@
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1762,7 +1773,7 @@
       <c r="L17" s="4">
         <v>16</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N17" s="4"/>
@@ -1776,19 +1787,19 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1819,19 +1830,19 @@
         <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1862,19 +1873,19 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1905,19 +1916,19 @@
         <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1948,19 +1959,19 @@
         <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1977,8 +1988,8 @@
       <c r="L22" s="4">
         <v>21</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>30</v>
+      <c r="M22" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>

</xml_diff>

<commit_message>
GUI PRE-PROTOTYPE v.1.2.0-0 (COMPLETE ver.)
21 basic card application.
</commit_message>
<xml_diff>
--- a/TestConsoleClient/TestConsoleClient/res/card.xlsx
+++ b/TestConsoleClient/TestConsoleClient/res/card.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>블랙퀸 해츨링</t>
   </si>
@@ -603,6 +603,10 @@
   </si>
   <si>
     <t>전장에 나와 있는 적군 중 하나를 아군으로 만든다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -614,7 +618,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -653,7 +657,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,12 +667,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -729,9 +727,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1037,11 +1032,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1057,7 +1052,7 @@
     <col min="18" max="18" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1104,7 +1099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1147,7 +1142,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1190,7 +1185,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1227,13 +1222,13 @@
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1276,7 +1271,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1319,7 +1314,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1362,7 +1357,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1399,13 +1394,13 @@
       <c r="L8" s="4">
         <v>7</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="24">
+    <row r="9" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1442,13 +1437,13 @@
       <c r="L9" s="4">
         <v>8</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>78</v>
+      <c r="M9" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1485,13 +1480,13 @@
       <c r="L10" s="4">
         <v>9</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1534,7 +1529,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="24">
+    <row r="12" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1577,7 +1572,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1620,7 +1615,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1663,7 +1658,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1706,7 +1701,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1744,12 +1739,12 @@
         <v>15</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1786,13 +1781,13 @@
       <c r="L17" s="4">
         <v>16</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="24">
+    <row r="18" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1835,7 +1830,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1878,7 +1873,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1915,13 +1910,13 @@
       <c r="L20" s="4">
         <v>19</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="7" t="s">
         <v>26</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="24">
+    <row r="21" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1964,7 +1959,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2001,7 +1996,7 @@
       <c r="L22" s="4">
         <v>21</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="7" t="s">
         <v>77</v>
       </c>
       <c r="N22" s="4"/>
@@ -2020,7 +2015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GUI PRE-PROTOTYPE v1.2.2-1 (used DataBase Server)
used DataBase Server
</commit_message>
<xml_diff>
--- a/TestConsoleClient/TestConsoleClient/res/card.xlsx
+++ b/TestConsoleClient/TestConsoleClient/res/card.xlsx
@@ -61,9 +61,6 @@
     <t>거대 좀비</t>
   </si>
   <si>
-    <t>거대 좀비가 전장에 입장한 턴 동안에는 상대방 마나 덱에 있는 마력을 마음 껏 사용할 수 있다.</t>
-  </si>
-  <si>
     <t>거인의 스켈레톤</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
   </si>
   <si>
     <t>악마의 열매</t>
-  </si>
-  <si>
-    <t>마력 카드를 1장 파괴해 원하는 상대에게 5의 데미지를 준다. 단, 파괴 될 마력 카드는 이 카드를 시동하기 위해 사용 될 수 없다.</t>
   </si>
   <si>
     <t>서큐버스 퀸의 유혹</t>
@@ -611,6 +605,14 @@
   </si>
   <si>
     <t>전장에서 카드가 하나 파괴 될 때마다 플레이어의 생명력이 +1 된다. 이효과는 이 카드가 파괴 될때까지 지속 되며 자기 자신의 파괴는 포함하지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거대 좀비가 전장에 입장한 턴 동안에는 상대방 마나 덱에 있는 마력을 마음 껏 사용할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마력 카드를 1장 파괴해 원하는 상대에게 5의 데미지를 준다. 단, 파괴 될 마력 카드는 이 카드를 시동하기 위해 사용 될 수 없다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -657,18 +659,12 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -726,7 +722,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1033,7 +1029,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1054,49 +1050,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1107,19 +1103,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -1137,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -1150,19 +1146,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1180,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1193,19 +1189,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -1222,7 +1218,7 @@
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="4"/>
@@ -1236,19 +1232,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1266,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1279,19 +1275,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -1309,7 +1305,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1319,22 +1315,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -1352,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1365,19 +1361,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -1394,7 +1390,7 @@
       <c r="L8" s="4">
         <v>7</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="N8" s="4"/>
@@ -1408,19 +1404,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1">
         <v>6</v>
@@ -1437,8 +1433,8 @@
       <c r="L9" s="4">
         <v>8</v>
       </c>
-      <c r="M9" s="7" t="s">
-        <v>79</v>
+      <c r="M9" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1451,19 +1447,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" s="1">
         <v>6</v>
@@ -1480,7 +1476,7 @@
       <c r="L10" s="4">
         <v>9</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="N10" s="4"/>
@@ -1494,19 +1490,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1524,7 +1520,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1537,19 +1533,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1">
         <v>5</v>
@@ -1566,8 +1562,8 @@
       <c r="L12" s="4">
         <v>11</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>13</v>
+      <c r="M12" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1577,22 +1573,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1610,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1620,22 +1616,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H14" s="1">
         <v>4</v>
@@ -1652,8 +1648,8 @@
       <c r="L14" s="4">
         <v>13</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>16</v>
+      <c r="M14" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1663,22 +1659,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H15" s="1">
         <v>3</v>
@@ -1696,7 +1692,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1706,22 +1702,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H16" s="1">
         <v>5</v>
@@ -1739,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1749,22 +1745,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1781,8 +1777,8 @@
       <c r="L17" s="4">
         <v>16</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>20</v>
+      <c r="M17" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1792,22 +1788,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1824,8 +1820,8 @@
       <c r="L18" s="4">
         <v>17</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>22</v>
+      <c r="M18" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1835,22 +1831,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1867,8 +1863,8 @@
       <c r="L19" s="4">
         <v>18</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>24</v>
+      <c r="M19" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1878,22 +1874,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1910,8 +1906,8 @@
       <c r="L20" s="4">
         <v>19</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>26</v>
+      <c r="M20" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1921,22 +1917,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1953,8 +1949,8 @@
       <c r="L21" s="4">
         <v>20</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>28</v>
+      <c r="M21" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1964,22 +1960,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1996,8 +1992,8 @@
       <c r="L22" s="4">
         <v>21</v>
       </c>
-      <c r="M22" s="7" t="s">
-        <v>77</v>
+      <c r="M22" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>

</xml_diff>

<commit_message>
DRAGON WARLORD GAME SINGLE PRE-PROTOTYPE FINAL VERSION (by. hae-kyung)
DRAGON WARLORD GAME SINGLE PRE-PROTOTYPE FINAL VERSION (by. hae-kyung)
</commit_message>
<xml_diff>
--- a/TestConsoleClient/TestConsoleClient/res/card.xlsx
+++ b/TestConsoleClient/TestConsoleClient/res/card.xlsx
@@ -61,6 +61,9 @@
     <t>거대 좀비</t>
   </si>
   <si>
+    <t>거대 좀비가 전장에 입장한 턴 동안에는 상대방 마나 덱에 있는 마력을 마음 껏 사용할 수 있다.</t>
+  </si>
+  <si>
     <t>거인의 스켈레톤</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
   </si>
   <si>
     <t>악마의 열매</t>
+  </si>
+  <si>
+    <t>마력 카드를 1장 파괴해 원하는 상대에게 5의 데미지를 준다. 단, 파괴 될 마력 카드는 이 카드를 시동하기 위해 사용 될 수 없다.</t>
   </si>
   <si>
     <t>서큐버스 퀸의 유혹</t>
@@ -605,14 +611,6 @@
   </si>
   <si>
     <t>전장에서 카드가 하나 파괴 될 때마다 플레이어의 생명력이 +1 된다. 이효과는 이 카드가 파괴 될때까지 지속 되며 자기 자신의 파괴는 포함하지 않는다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>거대 좀비가 전장에 입장한 턴 동안에는 상대방 마나 덱에 있는 마력을 마음 껏 사용할 수 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마력 카드를 1장 파괴해 원하는 상대에게 5의 데미지를 준다. 단, 파괴 될 마력 카드는 이 카드를 시동하기 위해 사용 될 수 없다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -659,12 +657,18 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -722,7 +726,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1029,7 +1033,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1050,49 +1054,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1103,19 +1107,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -1133,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -1146,19 +1150,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1176,7 +1180,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1189,19 +1193,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -1218,7 +1222,7 @@
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="4"/>
@@ -1232,19 +1236,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1262,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1275,19 +1279,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -1305,7 +1309,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1315,22 +1319,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -1348,7 +1352,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1361,19 +1365,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -1390,7 +1394,7 @@
       <c r="L8" s="4">
         <v>7</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N8" s="4"/>
@@ -1404,19 +1408,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" s="1">
         <v>6</v>
@@ -1433,8 +1437,8 @@
       <c r="L9" s="4">
         <v>8</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>77</v>
+      <c r="M9" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1447,19 +1451,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H10" s="1">
         <v>6</v>
@@ -1476,7 +1480,7 @@
       <c r="L10" s="4">
         <v>9</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="N10" s="4"/>
@@ -1490,19 +1494,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1520,7 +1524,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1533,19 +1537,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1">
         <v>5</v>
@@ -1562,8 +1566,8 @@
       <c r="L12" s="4">
         <v>11</v>
       </c>
-      <c r="M12" s="7" t="s">
-        <v>78</v>
+      <c r="M12" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1573,22 +1577,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1606,7 +1610,7 @@
         <v>12</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1616,22 +1620,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1">
         <v>4</v>
@@ -1648,8 +1652,8 @@
       <c r="L14" s="4">
         <v>13</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>15</v>
+      <c r="M14" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1659,22 +1663,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1">
         <v>3</v>
@@ -1692,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1702,22 +1706,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1">
         <v>5</v>
@@ -1735,7 +1739,7 @@
         <v>15</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1745,22 +1749,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1777,8 +1781,8 @@
       <c r="L17" s="4">
         <v>16</v>
       </c>
-      <c r="M17" s="6" t="s">
-        <v>19</v>
+      <c r="M17" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1788,22 +1792,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1820,8 +1824,8 @@
       <c r="L18" s="4">
         <v>17</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>21</v>
+      <c r="M18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1831,22 +1835,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1863,8 +1867,8 @@
       <c r="L19" s="4">
         <v>18</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>23</v>
+      <c r="M19" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1874,22 +1878,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1906,8 +1910,8 @@
       <c r="L20" s="4">
         <v>19</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>25</v>
+      <c r="M20" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1917,22 +1921,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1949,8 +1953,8 @@
       <c r="L21" s="4">
         <v>20</v>
       </c>
-      <c r="M21" s="7" t="s">
-        <v>79</v>
+      <c r="M21" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1960,22 +1964,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1992,8 +1996,8 @@
       <c r="L22" s="4">
         <v>21</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>75</v>
+      <c r="M22" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>

</xml_diff>